<commit_message>
Issue #1 : Petites retouches visuelles
</commit_message>
<xml_diff>
--- a/voitures.xlsx
+++ b/voitures.xlsx
@@ -46,7 +46,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="0" t="inlineStr">
@@ -133,6 +133,40 @@
         </is>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>Subaru</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>WRC Impreza GC</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>1997</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>Mitsubishi</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Lancer Evo IV</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>1997</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>